<commit_message>
Previous excavations data added
</commit_message>
<xml_diff>
--- a/tests/assets/tdd/spreadsheet/site.xlsx
+++ b/tests/assets/tdd/spreadsheet/site.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t xml:space="preserve">entry_id</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">ISL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some excavations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOMEONE2001</t>
   </si>
   <si>
     <t xml:space="preserve">Eleonora Quirico</t>
@@ -230,7 +236,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -370,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="6:6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R9" activeCellId="0" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -390,18 +396,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="68.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="43.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="37.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="75.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="39.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="35.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="44.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="36.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="29" style="1" width="11.57"/>
@@ -526,6 +532,12 @@
       <c r="Q2" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="T2" s="1" t="s">
         <v>34</v>
       </c>
@@ -542,7 +554,7 @@
         <v>32</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AA2" s="2" t="n">
         <v>43433</v>
@@ -550,7 +562,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>30</v>
@@ -562,37 +574,37 @@
         <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AA3" s="2" t="n">
         <v>43433</v>
@@ -600,13 +612,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>31</v>
@@ -615,7 +627,7 @@
         <v>32</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>34</v>
@@ -627,7 +639,7 @@
         <v>34</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>34</v>
@@ -645,7 +657,7 @@
         <v>34</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AA4" s="2" t="n">
         <v>43433</v>
@@ -653,13 +665,13 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>31</v>
@@ -668,7 +680,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>34</v>
@@ -680,7 +692,7 @@
         <v>34</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>34</v>
@@ -698,7 +710,7 @@
         <v>32</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AA5" s="2" t="n">
         <v>43433</v>
@@ -706,10 +718,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>31</v>
@@ -718,7 +730,7 @@
         <v>32</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>34</v>
@@ -730,7 +742,7 @@
         <v>34</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>34</v>
@@ -748,7 +760,7 @@
         <v>32</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AA6" s="2" t="n">
         <v>43433</v>

</xml_diff>